<commit_message>
Updated Digits Kinematics Length Data
</commit_message>
<xml_diff>
--- a/Analysis and Results/Digits Kinematics Data (mm).xlsx
+++ b/Analysis and Results/Digits Kinematics Data (mm).xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>DP_Length</t>
   </si>
@@ -91,6 +91,45 @@
   </si>
   <si>
     <t>MC_head_ligament_length (m)</t>
+  </si>
+  <si>
+    <t>DP_Length (mm)</t>
+  </si>
+  <si>
+    <t>MP_Length (mm)</t>
+  </si>
+  <si>
+    <t>PP_Length (mm)</t>
+  </si>
+  <si>
+    <t>MC_Lenght (mm)</t>
+  </si>
+  <si>
+    <t>IP_Joint_Radius (mm)</t>
+  </si>
+  <si>
+    <t>DIP_Joint_Radius (mm)</t>
+  </si>
+  <si>
+    <t>PIP_Joint_Radius (mm)</t>
+  </si>
+  <si>
+    <t>MCP_Joint_Radius (mm)</t>
+  </si>
+  <si>
+    <t>IP_Joint_Length (mm)</t>
+  </si>
+  <si>
+    <t>DIP_Joint_Length (mm)</t>
+  </si>
+  <si>
+    <t>PIP_Joint_Length (mm)</t>
+  </si>
+  <si>
+    <t>MCP_Joint_Length (mm)</t>
+  </si>
+  <si>
+    <t>MC_head_ligament_length (mm)</t>
   </si>
   <si>
     <t>DP_Length (mm)</t>
@@ -150,7 +189,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -161,15 +200,17 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -199,48 +240,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>14.120239233100833</v>
+        <v>29.360877984147542</v>
       </c>
       <c r="B2" s="0">
         <v>0</v>
@@ -281,7 +322,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>9.0332818510218083</v>
+        <v>21.110617731369206</v>
       </c>
       <c r="B3" s="0">
         <v>26.839804414339532</v>
@@ -322,7 +363,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>9.2571848182911438</v>
+        <v>20.401408548431156</v>
       </c>
       <c r="B4" s="0">
         <v>33.453482344891988</v>
@@ -363,7 +404,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>9.0228836853857306</v>
+        <v>20.154365035892347</v>
       </c>
       <c r="B5" s="0">
         <v>32.967473864401562</v>
@@ -404,7 +445,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>8.275710603930035</v>
+        <v>18.460373398173722</v>
       </c>
       <c r="B6" s="0">
         <v>24.749360945487059</v>

</xml_diff>